<commit_message>
Mises en forme mineures WS 02
</commit_message>
<xml_diff>
--- a/docs/base_de_donnees_materiaux/bdd_materiaux_v3.0 - sans prix -.xlsx
+++ b/docs/base_de_donnees_materiaux/bdd_materiaux_v3.0 - sans prix -.xlsx
@@ -1024,9 +1024,6 @@
     <t>pré-traité</t>
   </si>
   <si>
-    <t xml:space="preserve">Base de données Matériaux de l'IPOC AT-OMC v2.0 </t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1071,6 +1068,9 @@
       </rPr>
       <t xml:space="preserve"> Les éléments de l'usinabilité en gras sont des valeurs conformes trouvées dans le pdf "critère d'usinabilité", en revanche les valeurs en italiques sont des valeurs déterminées avec l'aide des valeurs connues d'autres materiaux et de la composition chimique.</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Base de données Matériaux de l'IPOC AT-OMC v3.0 </t>
   </si>
 </sst>
 </file>
@@ -2983,7 +2983,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:I16"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2993,7 +2993,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="224" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B1" s="224"/>
       <c r="C1" s="224"/>
@@ -3083,7 +3083,7 @@
     </row>
     <row r="9" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="225" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" s="225"/>
       <c r="C9" s="225"/>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="226" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B14" s="226"/>
       <c r="C14" s="226"/>
@@ -3193,12 +3193,12 @@
   <sheetPr codeName="Feuil2"/>
   <dimension ref="B1:AB79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D46" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="A6" sqref="A6"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3291,7 +3291,7 @@
       <c r="J5" s="107" t="s">
         <v>162</v>
       </c>
-      <c r="K5" s="113" t="s">
+      <c r="K5" s="135" t="s">
         <v>4</v>
       </c>
       <c r="L5" s="107" t="s">
@@ -9129,8 +9129,8 @@
   <sheetPr codeName="Feuil3"/>
   <dimension ref="B1:AC71"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="3" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="A6" sqref="A6"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>

</xml_diff>